<commit_message>
changes to optical system 3d model, new tests added to assembly instructions, changes to bom
</commit_message>
<xml_diff>
--- a/electronics/lia_bom.xlsx
+++ b/electronics/lia_bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="24915" windowHeight="12585"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12735" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="lia_bom" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="80">
   <si>
     <t>Comment</t>
   </si>
@@ -124,24 +124,12 @@
     <t>1206</t>
   </si>
   <si>
-    <t>MC7915</t>
-  </si>
-  <si>
-    <t>-15 V LDO regulator</t>
-  </si>
-  <si>
     <t>NREG</t>
   </si>
   <si>
     <t>D2PAK_L</t>
   </si>
   <si>
-    <t>MC78M15</t>
-  </si>
-  <si>
-    <t>+15 V LDO regulator</t>
-  </si>
-  <si>
     <t>PREG</t>
   </si>
   <si>
@@ -235,9 +223,6 @@
     <t>Cfy</t>
   </si>
   <si>
-    <t>AO3162</t>
-  </si>
-  <si>
     <t>NPN Bipolar Transistor</t>
   </si>
   <si>
@@ -257,6 +242,18 @@
   </si>
   <si>
     <t>(FUTURE USE - LEAVE OPEN)</t>
+  </si>
+  <si>
+    <t>MC7912</t>
+  </si>
+  <si>
+    <t>MC78M12</t>
+  </si>
+  <si>
+    <t>-12 V LDO regulator</t>
+  </si>
+  <si>
+    <t>+12 V LDO regulator</t>
   </si>
 </sst>
 </file>
@@ -623,7 +620,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -798,7 +795,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>32</v>
@@ -818,19 +815,19 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -838,19 +835,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -858,16 +855,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>35</v>
@@ -878,19 +875,19 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F13" s="3">
         <v>2</v>
@@ -898,19 +895,19 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F14" s="3">
         <v>7</v>
@@ -918,19 +915,19 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F15" s="3">
         <v>9</v>
@@ -938,19 +935,19 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F16" s="3">
         <v>9</v>
@@ -958,19 +955,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F17" s="3">
         <v>4</v>
@@ -978,19 +975,19 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F18" s="3">
         <v>2</v>
@@ -998,19 +995,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
@@ -1018,39 +1015,39 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F20" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2" t="s">
-        <v>73</v>
+      <c r="A21" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
@@ -1058,16 +1055,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>27</v>

</xml_diff>